<commit_message>
update correct Net 4 networks
</commit_message>
<xml_diff>
--- a/Adpated/Result.xlsx
+++ b/Adpated/Result.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlk/Desktop/Artificial Intelligence/3rd Year/Bayesian Networks/week3/Adpated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB9875B-5E5E-0A45-82E1-C18F8E4BDA7C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DB3651-9519-234D-AFF2-7947D1FE386B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DB84CAA0-3DCF-CB46-8FAD-DB5DD16BECCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$44:$A$49</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$44:$B$49</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$44:$B$49</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$44:$C$49</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$44:$C$49</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$44:$A$49</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$44:$B$49</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$44:$C$49</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$44:$A$49</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$44:$B$49</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$44:$C$49</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$44:$A$49</definedName>
-  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -171,7 +157,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1500"/>
-              <a:t>Amount of alternative representations per arrow count for network 2 </a:t>
+              <a:t>Amount of alternative representations per arrow count for network 3 </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -290,49 +276,73 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$23:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet1!$B$23:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AFCC-3742-8D48-0D1A1E9CCF61}"/>
+              <c16:uniqueId val="{00000000-6714-7D4F-B3AC-B321E73B5699}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -547,434 +557,6 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="1"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1500"/>
-              <a:t>Amount of alternative representations per arrow count for network 3 </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Networks</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="88500"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$23:$A$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$23:$B$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6714-7D4F-B3AC-B321E73B5699}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1567458272"/>
-        <c:axId val="1686528400"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1567458272"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1686528400"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1686528400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1567458272"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -1125,26 +707,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$44:$A$49</c:f>
+              <c:f>Sheet1!$A$44:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -1152,26 +737,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$44:$B$49</c:f>
+              <c:f>Sheet1!$B$44:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -1259,26 +847,29 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$44:$A$49</c:f>
+              <c:f>Sheet1!$A$44:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -1286,10 +877,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$44:$C$49</c:f>
+              <c:f>Sheet1!$C$44:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1306,6 +897,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
@@ -1314,6 +908,493 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-34D8-BA47-92CE-F09ACE4E393E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1320059104"/>
+        <c:axId val="1320035936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1320059104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320035936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1320035936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320059104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Amount of alternative representations per arrow count for network 2 </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Adapted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF97-DE48-A2CA-61A94E53D4B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EF97-DE48-A2CA-61A94E53D4B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1549,28 +1630,41 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
-  <a:schemeClr val="dk1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
   <cs:variation>
-    <a:tint val="88500"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="55000"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="75000"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="98500"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="30000"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="60000"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="80000"/>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -3128,42 +3222,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1517650</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC0AD45-FA2E-7B4E-AB46-03E4D138FE70}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -3194,7 +3252,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3202,16 +3260,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1511300</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3223,6 +3281,44 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D01C2E-310D-264B-B172-32E7412FA55C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3536,10 +3632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3DAD7-F3E9-6843-AA1F-1023F35B349C}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -3567,7 +3663,7 @@
       <c r="B2" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3576,9 +3672,9 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3587,9 +3683,9 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3600,7 +3696,7 @@
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>14</v>
       </c>
     </row>
@@ -3610,7 +3706,7 @@
       </c>
       <c r="B6" s="3">
         <f>SUM(B2:B5)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
@@ -3741,80 +3837,91 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="2">
-        <v>4</v>
-      </c>
-      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
-        <v>26</v>
-      </c>
-      <c r="C45" s="1">
+        <v>8</v>
+      </c>
+      <c r="C45" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="2">
-        <v>22</v>
-      </c>
-      <c r="C46" s="1">
+        <v>14</v>
+      </c>
+      <c r="C46" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
+        <v>7</v>
+      </c>
+      <c r="B47" s="2">
         <v>8</v>
       </c>
-      <c r="B47" s="2">
-        <v>16</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="2">
-        <v>10</v>
-      </c>
-      <c r="C48" s="1">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="2">
-        <v>20</v>
-      </c>
-      <c r="C49" s="1">
-        <v>120</v>
+        <v>2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2">
+        <v>10</v>
+      </c>
+      <c r="B50" s="2">
+        <v>20</v>
+      </c>
+      <c r="C50" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="3">
-        <f>SUM(B44:B49)</f>
-        <v>98</v>
-      </c>
-      <c r="C50" s="3">
-        <f>SUM(C44:C49)</f>
+      <c r="B51" s="3">
+        <f>SUM(B44:B50)</f>
+        <v>65</v>
+      </c>
+      <c r="C51" s="3">
+        <f>SUM(C44:C50)</f>
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed small bug in code and generated all network representations
</commit_message>
<xml_diff>
--- a/Adpated/Result.xlsx
+++ b/Adpated/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlk/Desktop/Artificial Intelligence/3rd Year/Bayesian Networks/week3/Adpated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F360BBE9-8479-1E4B-AE0D-E6DEB403CBBA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50992D1-F8C0-8243-8F84-45E1B1675FF8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DB84CAA0-3DCF-CB46-8FAD-DB5DD16BECCF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t xml:space="preserve"> Arrow Nr.</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Old Count</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>(mistake in the chart)</t>
   </si>
 </sst>
 </file>
@@ -123,434 +117,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="1"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1500"/>
-              <a:t>Amount of alternative representations per arrow count for network 3 </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Networks</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="88500"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$23:$A$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$23:$B$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6714-7D4F-B3AC-B321E73B5699}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1567458272"/>
-        <c:axId val="1686528400"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1567458272"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1686528400"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1686528400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1567458272"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -707,7 +273,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$44:$A$50</c:f>
+              <c:f>Sheet1!$A$42:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -737,7 +303,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$44:$B$50</c:f>
+              <c:f>Sheet1!$B$42:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -847,7 +413,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$44:$A$50</c:f>
+              <c:f>Sheet1!$A$42:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -877,7 +443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$44:$C$50</c:f>
+              <c:f>Sheet1!$C$42:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -908,6 +474,493 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-34D8-BA47-92CE-F09ACE4E393E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1320059104"/>
+        <c:axId val="1320035936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1320059104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320035936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1320035936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320059104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Amount of alternative representations per arrow count for network 2 </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Adapted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF97-DE48-A2CA-61A94E53D4B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Original</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EF97-DE48-A2CA-61A94E53D4B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1152,7 +1205,7 @@
               <a:rPr lang="en-US" sz="1500" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Amount of alternative representations per arrow count for network 2 </a:t>
+              <a:t>Amount of alternative representations per arrow count for network 3 </a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1500">
               <a:effectLst/>
@@ -1270,30 +1323,63 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet1!$B$23:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EF97-DE48-A2CA-61A94E53D4B9}"/>
+              <c16:uniqueId val="{00000000-A0CD-9742-AB02-8DA5BF4F8A1A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1371,30 +1457,63 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>Sheet1!$C$23:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EF97-DE48-A2CA-61A94E53D4B9}"/>
+              <c16:uniqueId val="{00000001-A0CD-9742-AB02-8DA5BF4F8A1A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1603,28 +1722,41 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
-  <a:schemeClr val="dk1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
   <cs:variation>
-    <a:tint val="88500"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="55000"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="75000"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="98500"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="30000"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="60000"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:tint val="80000"/>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -3224,51 +3356,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDC8840-2AB1-0444-80CC-FDD6EA0885B3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3288,7 +3382,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3313,6 +3407,44 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D01C2E-310D-264B-B172-32E7412FA55C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35BA5E9D-9302-0C4E-ADEA-88F56457B40A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3632,10 +3764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3DAD7-F3E9-6843-AA1F-1023F35B349C}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -3726,121 +3858,122 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
         <v>4</v>
       </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
+      <c r="C23" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C24" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2">
-        <v>12</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="C25" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>24</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C27" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="C28" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>10</v>
-      </c>
-      <c r="B29" s="2">
-        <v>20</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
+      <c r="A29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3">
+        <f>SUM(B23:B28)</f>
+        <v>74</v>
+      </c>
+      <c r="C29" s="3">
+        <f>SUM(C23:C28)</f>
+        <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>11</v>
-      </c>
-      <c r="B30" s="2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="3">
-        <f>SUM(B23:B30)</f>
-        <v>99</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="2">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2">
+        <v>8</v>
+      </c>
+      <c r="C43" s="2">
         <v>0</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B44" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C44" s="2">
         <v>0</v>
@@ -3848,7 +3981,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B45" s="2">
         <v>8</v>
@@ -3859,10 +3992,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C46" s="2">
         <v>0</v>
@@ -3870,10 +4003,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -3881,47 +4014,25 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="2">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C48" s="2">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>9</v>
-      </c>
-      <c r="B49" s="2">
+      <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>10</v>
-      </c>
-      <c r="B50" s="2">
-        <v>20</v>
-      </c>
-      <c r="C50" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="3">
-        <f>SUM(B44:B50)</f>
+      <c r="B49" s="3">
+        <f>SUM(B42:B48)</f>
         <v>65</v>
       </c>
-      <c r="C51" s="3">
-        <f>SUM(C44:C50)</f>
+      <c r="C49" s="3">
+        <f>SUM(C42:C48)</f>
         <v>120</v>
       </c>
     </row>

</xml_diff>